<commit_message>
Added mail changes and in config.properties file
</commit_message>
<xml_diff>
--- a/src/main/resources/testdatasheets/TestCredentials.xlsx
+++ b/src/main/resources/testdatasheets/TestCredentials.xlsx
@@ -48,13 +48,13 @@
     <t>CC - Mail Ids</t>
   </si>
   <si>
-    <t>mtbxcbhrhbycngce</t>
-  </si>
-  <si>
     <t>shivanshusingla82@gmail.com</t>
   </si>
   <si>
     <t>shubham.patel@grofers.com</t>
+  </si>
+  <si>
+    <t>dlkzgzdeizmgpqje</t>
   </si>
 </sst>
 </file>
@@ -525,10 +525,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -575,10 +575,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>